<commit_message>
ébauche page de mots + ajout et suppr des données
</commit_message>
<xml_diff>
--- a/traductions/traduction_fr.xlsx
+++ b/traductions/traduction_fr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Lexique/Etude/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Projet/traductions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70CC773E-9707-44DF-96A0-FB821E7242C3}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B2632A-C45E-4878-9098-1ECFF672A5AD}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -280,6 +280,42 @@
   </si>
   <si>
     <t>Choisir les fichiers</t>
+  </si>
+  <si>
+    <t>synonyme</t>
+  </si>
+  <si>
+    <t>Synonymes :</t>
+  </si>
+  <si>
+    <t>origine</t>
+  </si>
+  <si>
+    <t>Origines géographiques :</t>
+  </si>
+  <si>
+    <t>pron</t>
+  </si>
+  <si>
+    <t>Prononciation :</t>
+  </si>
+  <si>
+    <t>theme</t>
+  </si>
+  <si>
+    <t>Thématiques :</t>
+  </si>
+  <si>
+    <t>exemple</t>
+  </si>
+  <si>
+    <t>Exemples :</t>
+  </si>
+  <si>
+    <t>etymo</t>
+  </si>
+  <si>
+    <t>Etymologie :</t>
   </si>
 </sst>
 </file>
@@ -334,13 +370,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B45" totalsRowShown="0">
-  <autoFilter ref="A1:B45" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B51" totalsRowShown="0">
+  <autoFilter ref="A1:B51" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C3E67EDD-C069-4699-9F96-F2EDC31EF19F}" name="ID"/>
     <tableColumn id="2" xr3:uid="{37BD1132-CE7D-4C7F-AD78-D3026F5A9F46}" name="valeur"/>
@@ -646,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE7F0C-CEF0-4290-823D-748F682C320F}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1057,54 @@
         <v>81</v>
       </c>
     </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bouton déco et bouton administration fonctionnels
</commit_message>
<xml_diff>
--- a/traductions/traduction_fr.xlsx
+++ b/traductions/traduction_fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Projet/traductions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B2632A-C45E-4878-9098-1ECFF672A5AD}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C39780-7C8E-4003-817D-47D2780D49B0}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -316,6 +316,24 @@
   </si>
   <si>
     <t>Etymologie :</t>
+  </si>
+  <si>
+    <t>login-button_connecte</t>
+  </si>
+  <si>
+    <t>bouton_admin</t>
+  </si>
+  <si>
+    <t>bouton_deco</t>
+  </si>
+  <si>
+    <t>Page d'administration</t>
+  </si>
+  <si>
+    <t>Se déconnecter</t>
+  </si>
+  <si>
+    <t>Connecté</t>
   </si>
 </sst>
 </file>
@@ -370,9 +388,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B51" totalsRowShown="0">
-  <autoFilter ref="A1:B51" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B54" totalsRowShown="0">
+  <autoFilter ref="A1:B54" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C3E67EDD-C069-4699-9F96-F2EDC31EF19F}" name="ID"/>
     <tableColumn id="2" xr3:uid="{37BD1132-CE7D-4C7F-AD78-D3026F5A9F46}" name="valeur"/>
@@ -678,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE7F0C-CEF0-4290-823D-748F682C320F}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,6 +1127,30 @@
         <v>96</v>
       </c>
     </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
nb résultats + corrections affichage
</commit_message>
<xml_diff>
--- a/traductions/traduction_fr.xlsx
+++ b/traductions/traduction_fr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Projet/traductions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C39780-7C8E-4003-817D-47D2780D49B0}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{268B1714-ACE8-459A-894C-A6C77C6295B0}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
   </bookViews>
   <sheets>
     <sheet name="fr" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>titre_resultats</t>
   </si>
   <si>
-    <t> Résultats pour le mot " x " :</t>
-  </si>
-  <si>
     <t>mots_similaires</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>Connecté</t>
+  </si>
+  <si>
+    <t> Résultats :</t>
   </si>
 </sst>
 </file>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE7F0C-CEF0-4290-823D-748F682C320F}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,10 +721,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,15 +844,15 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
         <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -860,295 +860,295 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
         <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
         <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
         <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
         <v>51</v>
-      </c>
-      <c r="B27" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
         <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
         <v>59</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
         <v>61</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
-      </c>
-      <c r="B33" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
         <v>65</v>
-      </c>
-      <c r="B34" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
         <v>69</v>
-      </c>
-      <c r="B36" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
         <v>76</v>
-      </c>
-      <c r="B41" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
         <v>80</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
         <v>85</v>
-      </c>
-      <c r="B46" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
         <v>87</v>
-      </c>
-      <c r="B47" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
         <v>89</v>
-      </c>
-      <c r="B48" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" t="s">
         <v>91</v>
-      </c>
-      <c r="B49" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" t="s">
         <v>93</v>
-      </c>
-      <c r="B50" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" t="s">
         <v>95</v>
-      </c>
-      <c r="B51" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
téléchargement des représentations de ressource
</commit_message>
<xml_diff>
--- a/traductions/traduction_fr.xlsx
+++ b/traductions/traduction_fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Projet/traductions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{268B1714-ACE8-459A-894C-A6C77C6295B0}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF7ADFB8-90C9-48A5-A054-4E7D108F7879}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t> Résultats :</t>
+  </si>
+  <si>
+    <t>export_data_btn</t>
+  </si>
+  <si>
+    <t>Télécharger</t>
   </si>
 </sst>
 </file>
@@ -393,8 +399,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B54" totalsRowShown="0">
-  <autoFilter ref="A1:B54" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B55" totalsRowShown="0">
+  <autoFilter ref="A1:B55" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C3E67EDD-C069-4699-9F96-F2EDC31EF19F}" name="ID"/>
     <tableColumn id="2" xr3:uid="{37BD1132-CE7D-4C7F-AD78-D3026F5A9F46}" name="valeur"/>
@@ -700,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE7F0C-CEF0-4290-823D-748F682C320F}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,6 +1157,14 @@
         <v>100</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
styling + corrections mineures
</commit_message>
<xml_diff>
--- a/traductions/traduction_fr.xlsx
+++ b/traductions/traduction_fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Projet/traductions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF7ADFB8-90C9-48A5-A054-4E7D108F7879}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6A6076A-4177-4AC6-9D9B-32B782F44F3F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>ID</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>Télécharger</t>
+  </si>
+  <si>
+    <t>msg_btn</t>
+  </si>
+  <si>
+    <t>Envoyer le message</t>
   </si>
 </sst>
 </file>
@@ -399,8 +405,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B55" totalsRowShown="0">
-  <autoFilter ref="A1:B55" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B56" totalsRowShown="0">
+  <autoFilter ref="A1:B56" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C3E67EDD-C069-4699-9F96-F2EDC31EF19F}" name="ID"/>
     <tableColumn id="2" xr3:uid="{37BD1132-CE7D-4C7F-AD78-D3026F5A9F46}" name="valeur"/>
@@ -706,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE7F0C-CEF0-4290-823D-748F682C320F}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,6 +1171,14 @@
         <v>104</v>
       </c>
     </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
afichage contacts + corrections
</commit_message>
<xml_diff>
--- a/traductions/traduction_fr.xlsx
+++ b/traductions/traduction_fr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Projet/traductions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27166919-F721-4B6D-A50F-BF7779DF1F2F}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A20F85E-A86D-495E-A66D-15BE91760D07}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="2625" windowWidth="21600" windowHeight="11385" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
+    <workbookView xWindow="13860" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
   </bookViews>
   <sheets>
     <sheet name="fr" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -388,6 +388,75 @@
   </si>
   <si>
     <t>Aucun</t>
+  </si>
+  <si>
+    <t>contact_msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merci d'avoir pris le temps de nous contacter ! </t>
+  </si>
+  <si>
+    <t>unauth_err</t>
+  </si>
+  <si>
+    <t>Vous n'êtes pas connecté(e) !</t>
+  </si>
+  <si>
+    <t>deco_msg</t>
+  </si>
+  <si>
+    <t>Vous avez bien été déconnecté.</t>
+  </si>
+  <si>
+    <t>badreq_err</t>
+  </si>
+  <si>
+    <t>Mauvaise requête.</t>
+  </si>
+  <si>
+    <t>co_msg</t>
+  </si>
+  <si>
+    <t>Connecté(e) !</t>
+  </si>
+  <si>
+    <t>contact_err</t>
+  </si>
+  <si>
+    <t>Il y a eu une erreur en traitant votre demande.</t>
+  </si>
+  <si>
+    <t>upload_msg</t>
+  </si>
+  <si>
+    <t>Import réussi !</t>
+  </si>
+  <si>
+    <t>contact_nom</t>
+  </si>
+  <si>
+    <t>contact_sujet</t>
+  </si>
+  <si>
+    <t>contact_mail</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Objet</t>
+  </si>
+  <si>
+    <t>Adresse mail</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>contact_corps</t>
+  </si>
+  <si>
+    <t>contact_suppr</t>
   </si>
 </sst>
 </file>
@@ -447,8 +516,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B63" totalsRowShown="0">
-  <autoFilter ref="A1:B63" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B75" totalsRowShown="0">
+  <autoFilter ref="A1:B75" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C3E67EDD-C069-4699-9F96-F2EDC31EF19F}" name="ID"/>
     <tableColumn id="2" xr3:uid="{37BD1132-CE7D-4C7F-AD78-D3026F5A9F46}" name="valeur"/>
@@ -754,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE7F0C-CEF0-4290-823D-748F682C320F}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,6 +1346,102 @@
         <v>120</v>
       </c>
     </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
trad + fix bug longs fichiers
</commit_message>
<xml_diff>
--- a/traductions/traduction_fr.xlsx
+++ b/traductions/traduction_fr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a79823e041745b72/Documents/VIE ETUDIANTE/2023-2024/Cours/Projet Pro/Projet/traductions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A20F85E-A86D-495E-A66D-15BE91760D07}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="13_ncr:1_{85E6B19F-9A9D-4A04-A965-B036DF56B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{250371A8-9D82-4B34-85BB-7AD794FEEE25}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="3000" windowWidth="21600" windowHeight="11385" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
+    <workbookView xWindow="2760" yWindow="2880" windowWidth="21600" windowHeight="11385" xr2:uid="{0304B7E8-873D-4A0E-91CD-5A66F8A041E8}"/>
   </bookViews>
   <sheets>
     <sheet name="fr" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="146">
   <si>
     <t>ID</t>
   </si>
@@ -457,6 +457,12 @@
   </si>
   <si>
     <t>contact_suppr</t>
+  </si>
+  <si>
+    <t>donnees_recues</t>
+  </si>
+  <si>
+    <t>Contacts</t>
   </si>
 </sst>
 </file>
@@ -516,8 +522,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B75" totalsRowShown="0">
-  <autoFilter ref="A1:B75" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}" name="Traductions" displayName="Traductions" ref="A1:B76" totalsRowShown="0">
+  <autoFilter ref="A1:B76" xr:uid="{2625E90A-DCC3-4F51-83F9-F00420EB653D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C3E67EDD-C069-4699-9F96-F2EDC31EF19F}" name="ID"/>
     <tableColumn id="2" xr3:uid="{37BD1132-CE7D-4C7F-AD78-D3026F5A9F46}" name="valeur"/>
@@ -823,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BE7F0C-CEF0-4290-823D-748F682C320F}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,6 +1448,14 @@
         <v>67</v>
       </c>
     </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>144</v>
+      </c>
+      <c r="B76" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>